<commit_message>
Misc Changes, and OMIT R20 to fix SDA tied to A4 issue
</commit_message>
<xml_diff>
--- a/BOM V1/BOM_DigiKey_Order_11.23.18.xlsx
+++ b/BOM V1/BOM_DigiKey_Order_11.23.18.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\MIT\Fall 2018\FLAPS\KiCad Design\SMA_Driver_V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\MIT\Fall 2018\FLAPS\KiCad Design\SMA_Driver_V1\BOM V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F0D682-65D6-40C1-A1CF-6BD4C1A76D1B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB647F01-2EA0-4882-B73E-04AE369AA816}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>